<commit_message>
This commit and push is for synchronizing the works and show the current result to the interviewer
</commit_message>
<xml_diff>
--- a/saving file/705.xlsx
+++ b/saving file/705.xlsx
@@ -7657,38 +7657,42 @@
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>C11H22</t>
-        </is>
-      </c>
-      <c r="I115" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J115" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K115" t="inlineStr">
         <is>
-          <t>Olefin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L115" t="inlineStr">
         <is>
-          <t>Olefin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M115" t="inlineStr">
         <is>
-          <t>Olefin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>Olefin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
         <is>
-          <t>Olefin</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -7720,38 +7724,42 @@
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>C11H10FNS</t>
-        </is>
-      </c>
-      <c r="I116" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K116" t="inlineStr">
         <is>
-          <t>Heteroatomic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L116" t="inlineStr">
         <is>
-          <t>Di-Aromatic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M116" t="inlineStr">
         <is>
-          <t>Aromatic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -7783,38 +7791,42 @@
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>C11H22</t>
-        </is>
-      </c>
-      <c r="I117" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J117" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K117" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L117" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M117" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -7846,38 +7858,42 @@
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>C15H24F6O2</t>
-        </is>
-      </c>
-      <c r="I118" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J118" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K118" t="inlineStr">
         <is>
-          <t>Heteroatomic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L118" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M118" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N118" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O118" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -7909,38 +7925,42 @@
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>C8H5N3O4</t>
-        </is>
-      </c>
-      <c r="I119" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J119" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K119" t="inlineStr">
         <is>
-          <t>Heteroatomic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L119" t="inlineStr">
         <is>
-          <t>Mono-Aromatic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M119" t="inlineStr">
         <is>
-          <t>Aromatic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N119" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O119" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -7972,38 +7992,42 @@
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>C12H22</t>
-        </is>
-      </c>
-      <c r="I120" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J120" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K120" t="inlineStr">
         <is>
-          <t>Olefin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L120" t="inlineStr">
         <is>
-          <t>Olefin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M120" t="inlineStr">
         <is>
-          <t>Olefin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>Olefin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O120" t="inlineStr">
         <is>
-          <t>Olefin</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8035,38 +8059,42 @@
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>C6H18O3Si3</t>
-        </is>
-      </c>
-      <c r="I121" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J121" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K121" t="inlineStr">
         <is>
-          <t>Heteroatomic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L121" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M121" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8098,38 +8126,42 @@
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>C12H24</t>
-        </is>
-      </c>
-      <c r="I122" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J122" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K122" t="inlineStr">
         <is>
-          <t>Olefin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L122" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M122" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8161,38 +8193,42 @@
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>C15H28</t>
-        </is>
-      </c>
-      <c r="I123" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J123" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K123" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L123" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M123" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N123" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O123" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8224,38 +8260,42 @@
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>C12H26</t>
-        </is>
-      </c>
-      <c r="I124" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J124" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K124" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L124" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M124" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8287,38 +8327,42 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>C8H5N3O4</t>
-        </is>
-      </c>
-      <c r="I125" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J125" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K125" t="inlineStr">
         <is>
-          <t>Heteroatomic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L125" t="inlineStr">
         <is>
-          <t>Di-Aromatic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>Aromatic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8350,38 +8394,42 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>C8H5N3O4</t>
-        </is>
-      </c>
-      <c r="I126" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J126" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K126" t="inlineStr">
         <is>
-          <t>Heteroatomic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L126" t="inlineStr">
         <is>
-          <t>Di-Aromatic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M126" t="inlineStr">
         <is>
-          <t>Aromatic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O126" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8413,38 +8461,42 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>C13H26</t>
-        </is>
-      </c>
-      <c r="I127" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J127" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K127" t="inlineStr">
         <is>
-          <t>Olefin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L127" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M127" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8476,38 +8528,42 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>C13H28</t>
-        </is>
-      </c>
-      <c r="I128" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J128" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K128" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M128" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8539,38 +8595,42 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>C12H36O6Si6</t>
-        </is>
-      </c>
-      <c r="I129" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J129" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K129" t="inlineStr">
         <is>
-          <t>Heteroatomic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M129" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8602,38 +8662,42 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>C14H28</t>
-        </is>
-      </c>
-      <c r="I130" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J130" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K130" t="inlineStr">
         <is>
-          <t>Olefin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L130" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M130" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8665,38 +8729,42 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>C20H42</t>
-        </is>
-      </c>
-      <c r="I131" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J131" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K131" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L131" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M131" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8728,38 +8796,42 @@
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>C14H42O7Si7</t>
-        </is>
-      </c>
-      <c r="I132" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J132" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K132" t="inlineStr">
         <is>
-          <t>Heteroatomic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L132" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M132" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N132" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O132" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8791,38 +8863,42 @@
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>C15H30</t>
-        </is>
-      </c>
-      <c r="I133" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J133" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K133" t="inlineStr">
         <is>
-          <t>Olefin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L133" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8854,38 +8930,42 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>C15H32</t>
-        </is>
-      </c>
-      <c r="I134" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J134" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K134" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L134" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8917,38 +8997,42 @@
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>C6H18O3Si3</t>
-        </is>
-      </c>
-      <c r="I135" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K135" t="inlineStr">
         <is>
-          <t>Heteroatomic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L135" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>Naphthene</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -8980,38 +9064,42 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>C22H46</t>
-        </is>
-      </c>
-      <c r="I136" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J136" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>Paraffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L136" t="inlineStr">
         <is>
-          <t>Isoparaffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>Isoparaffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N136" t="inlineStr">
         <is>
-          <t>Isoparaffin</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O136" t="inlineStr">
         <is>
-          <t>Isoparaffin</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>
@@ -9043,38 +9131,42 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>C20H42O4Si4</t>
-        </is>
-      </c>
-      <c r="I137" t="inlineStr"/>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="K137" t="inlineStr">
         <is>
-          <t>Heteroatomic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="L137" t="inlineStr">
         <is>
-          <t>Mono-Aromatic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="M137" t="inlineStr">
         <is>
-          <t>Aromatic</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="N137" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="O137" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Not Found</t>
         </is>
       </c>
     </row>

</xml_diff>